<commit_message>
Update xlsx default form for health facility by integrating select multiple field
</commit_message>
<xml_diff>
--- a/setuper/data/default_Health_facility_form.xlsx
+++ b/setuper/data/default_Health_facility_form.xlsx
@@ -206,7 +206,7 @@
     <t xml:space="preserve">Is there electricity at the health facility?</t>
   </si>
   <si>
-    <t xml:space="preserve">select_one source_electricite</t>
+    <t xml:space="preserve">select_multiple source_electricite</t>
   </si>
   <si>
     <t xml:space="preserve">HFR_CS_17</t>
@@ -221,7 +221,7 @@
     <t xml:space="preserve">${HFR_CS_16}='yes'</t>
   </si>
   <si>
-    <t xml:space="preserve">select_one source_eau</t>
+    <t xml:space="preserve">select_multiple source_eau</t>
   </si>
   <si>
     <t xml:space="preserve">HFR_CS_18</t>
@@ -846,7 +846,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -871,10 +871,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -883,11 +879,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1031,12 +1027,12 @@
   <dimension ref="A1:AH978"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+      <selection pane="bottomLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.45"/>
@@ -1096,637 +1092,588 @@
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="0" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="6" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-    </row>
-    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="6"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-    </row>
+    </row>
+    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="0" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="F8" s="6"/>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="6"/>
-      <c r="I9" s="6"/>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="E10" s="6"/>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E11" s="6"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="9"/>
-      <c r="L11" s="9"/>
-      <c r="M11" s="9"/>
-      <c r="N11" s="9"/>
-      <c r="O11" s="9"/>
-      <c r="P11" s="9"/>
-      <c r="Q11" s="9"/>
-      <c r="R11" s="9"/>
-      <c r="S11" s="9"/>
-      <c r="T11" s="9"/>
-      <c r="U11" s="9"/>
-      <c r="V11" s="9"/>
-      <c r="W11" s="9"/>
-      <c r="X11" s="9"/>
-      <c r="Y11" s="9"/>
-      <c r="Z11" s="9"/>
-      <c r="AA11" s="9"/>
-      <c r="AB11" s="9"/>
-      <c r="AC11" s="9"/>
-      <c r="AD11" s="9"/>
-      <c r="AE11" s="9"/>
-      <c r="AF11" s="9"/>
-      <c r="AG11" s="9"/>
-      <c r="AH11" s="9"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
+      <c r="M11" s="8"/>
+      <c r="N11" s="8"/>
+      <c r="O11" s="8"/>
+      <c r="P11" s="8"/>
+      <c r="Q11" s="8"/>
+      <c r="R11" s="8"/>
+      <c r="S11" s="8"/>
+      <c r="T11" s="8"/>
+      <c r="U11" s="8"/>
+      <c r="V11" s="8"/>
+      <c r="W11" s="8"/>
+      <c r="X11" s="8"/>
+      <c r="Y11" s="8"/>
+      <c r="Z11" s="8"/>
+      <c r="AA11" s="8"/>
+      <c r="AB11" s="8"/>
+      <c r="AC11" s="8"/>
+      <c r="AD11" s="8"/>
+      <c r="AE11" s="8"/>
+      <c r="AF11" s="8"/>
+      <c r="AG11" s="8"/>
+      <c r="AH11" s="8"/>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="D12" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="E12" s="6"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="9"/>
-      <c r="L12" s="9"/>
-      <c r="M12" s="9"/>
-      <c r="N12" s="9"/>
-      <c r="O12" s="9"/>
-      <c r="P12" s="9"/>
-      <c r="Q12" s="9"/>
-      <c r="R12" s="9"/>
-      <c r="S12" s="9"/>
-      <c r="T12" s="9"/>
-      <c r="U12" s="9"/>
-      <c r="V12" s="9"/>
-      <c r="W12" s="9"/>
-      <c r="X12" s="9"/>
-      <c r="Y12" s="9"/>
-      <c r="Z12" s="9"/>
-      <c r="AA12" s="9"/>
-      <c r="AB12" s="9"/>
-      <c r="AC12" s="9"/>
-      <c r="AD12" s="9"/>
-      <c r="AE12" s="9"/>
-      <c r="AF12" s="9"/>
-      <c r="AG12" s="9"/>
-      <c r="AH12" s="9"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="8"/>
+      <c r="O12" s="8"/>
+      <c r="P12" s="8"/>
+      <c r="Q12" s="8"/>
+      <c r="R12" s="8"/>
+      <c r="S12" s="8"/>
+      <c r="T12" s="8"/>
+      <c r="U12" s="8"/>
+      <c r="V12" s="8"/>
+      <c r="W12" s="8"/>
+      <c r="X12" s="8"/>
+      <c r="Y12" s="8"/>
+      <c r="Z12" s="8"/>
+      <c r="AA12" s="8"/>
+      <c r="AB12" s="8"/>
+      <c r="AC12" s="8"/>
+      <c r="AD12" s="8"/>
+      <c r="AE12" s="8"/>
+      <c r="AF12" s="8"/>
+      <c r="AG12" s="8"/>
+      <c r="AH12" s="8"/>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="E13" s="6"/>
-      <c r="I13" s="6"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="0" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="11"/>
-      <c r="B15" s="11"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="6"/>
-      <c r="K15" s="7"/>
-      <c r="L15" s="6"/>
-      <c r="M15" s="6"/>
-      <c r="N15" s="6"/>
-      <c r="O15" s="6"/>
-      <c r="P15" s="6"/>
-      <c r="Q15" s="6"/>
-      <c r="R15" s="6"/>
-      <c r="S15" s="6"/>
-      <c r="T15" s="6"/>
-      <c r="U15" s="6"/>
-      <c r="V15" s="6"/>
-      <c r="W15" s="6"/>
-      <c r="X15" s="6"/>
-      <c r="Y15" s="6"/>
-      <c r="Z15" s="6"/>
-      <c r="AA15" s="6"/>
-      <c r="AB15" s="6"/>
-      <c r="AC15" s="6"/>
-      <c r="AD15" s="6"/>
-      <c r="AE15" s="6"/>
-      <c r="AF15" s="6"/>
-      <c r="AG15" s="6"/>
-      <c r="AH15" s="6"/>
+      <c r="A15" s="10"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="K15" s="6"/>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="0" t="s">
         <v>51</v>
       </c>
-      <c r="F16" s="6" t="s">
+      <c r="F16" s="0" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="D17" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="F17" s="6"/>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="13" t="s">
+      <c r="A18" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="B18" s="14" t="s">
+      <c r="B18" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="C18" s="15" t="s">
+      <c r="C18" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="D18" s="13" t="s">
+      <c r="D18" s="12" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="13" t="s">
+      <c r="A19" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="B19" s="13" t="s">
+      <c r="B19" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="C19" s="15" t="s">
+      <c r="C19" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="D19" s="13" t="s">
+      <c r="D19" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="I19" s="16" t="s">
+      <c r="I19" s="15" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="13" t="s">
+      <c r="A20" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="B20" s="13" t="s">
+      <c r="B20" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="C20" s="15" t="s">
+      <c r="C20" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="D20" s="13" t="s">
+      <c r="D20" s="12" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="13" t="s">
+      <c r="A21" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="13"/>
-      <c r="C21" s="15"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="14"/>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="13"/>
-      <c r="B22" s="13"/>
-      <c r="C22" s="15"/>
+      <c r="A22" s="12"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="14"/>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="B23" s="13" t="s">
+      <c r="B23" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="C23" s="15" t="s">
+      <c r="C23" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="D23" s="6" t="s">
+      <c r="D23" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="F23" s="6" t="s">
+      <c r="F23" s="0" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="13" t="s">
+      <c r="A24" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B24" s="13" t="s">
+      <c r="B24" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="C24" s="17" t="s">
+      <c r="C24" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="D24" s="8" t="s">
+      <c r="D24" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="F24" s="6"/>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="13" t="s">
+      <c r="A25" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="B25" s="13" t="s">
+      <c r="B25" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="C25" s="15" t="s">
+      <c r="C25" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="D25" s="0" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="13" t="s">
+      <c r="A26" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="B26" s="13" t="s">
+      <c r="B26" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="C26" s="15" t="s">
+      <c r="C26" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="D26" s="6" t="s">
+      <c r="D26" s="0" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="13" t="s">
+      <c r="A27" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="B27" s="13" t="s">
+      <c r="B27" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="C27" s="15" t="s">
+      <c r="C27" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="D27" s="0" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="13" t="s">
+      <c r="A28" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="B28" s="13" t="s">
+      <c r="B28" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="C28" s="15" t="s">
+      <c r="C28" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="D28" s="6" t="s">
+      <c r="D28" s="0" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="13" t="s">
+      <c r="A29" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="B29" s="13" t="s">
+      <c r="B29" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="C29" s="15" t="s">
+      <c r="C29" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="D29" s="6" t="s">
+      <c r="D29" s="0" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="13" t="s">
+      <c r="A30" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="B30" s="13" t="s">
+      <c r="B30" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="C30" s="15" t="s">
+      <c r="C30" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="D30" s="6" t="s">
+      <c r="D30" s="0" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="6" t="s">
+      <c r="A31" s="0" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="6" t="s">
+      <c r="A33" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="B33" s="0" t="s">
         <v>88</v>
       </c>
-      <c r="C33" s="6" t="s">
+      <c r="C33" s="0" t="s">
         <v>89</v>
       </c>
-      <c r="D33" s="6" t="s">
+      <c r="D33" s="0" t="s">
         <v>90</v>
       </c>
-      <c r="F33" s="6" t="s">
+      <c r="F33" s="0" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="18" t="s">
+      <c r="A34" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="B34" s="18" t="s">
+      <c r="B34" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="C34" s="8" t="s">
+      <c r="C34" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="D34" s="8" t="s">
+      <c r="D34" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="F34" s="6"/>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="13" t="s">
+      <c r="A35" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="B35" s="13" t="s">
+      <c r="B35" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="C35" s="13" t="s">
+      <c r="C35" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="D35" s="13" t="s">
+      <c r="D35" s="12" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="13" t="s">
+      <c r="A36" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="B36" s="13" t="s">
+      <c r="B36" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="C36" s="13" t="s">
+      <c r="C36" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="D36" s="13" t="s">
+      <c r="D36" s="12" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="13" t="s">
+      <c r="A37" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="B37" s="13" t="s">
+      <c r="B37" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="C37" s="13" t="s">
+      <c r="C37" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="D37" s="13" t="s">
+      <c r="D37" s="12" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="13" t="s">
+      <c r="A38" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="B38" s="13" t="s">
+      <c r="B38" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="C38" s="13"/>
-      <c r="D38" s="13"/>
-      <c r="M38" s="19" t="s">
+      <c r="C38" s="12"/>
+      <c r="D38" s="12"/>
+      <c r="M38" s="18" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="13" t="s">
+      <c r="A39" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="B39" s="13" t="s">
+      <c r="B39" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="C39" s="13"/>
-      <c r="D39" s="13"/>
-      <c r="E39" s="13"/>
-      <c r="F39" s="13"/>
-      <c r="G39" s="13"/>
-      <c r="H39" s="13"/>
-      <c r="I39" s="13"/>
-      <c r="M39" s="19" t="s">
+      <c r="C39" s="12"/>
+      <c r="D39" s="12"/>
+      <c r="E39" s="12"/>
+      <c r="F39" s="12"/>
+      <c r="G39" s="12"/>
+      <c r="H39" s="12"/>
+      <c r="I39" s="12"/>
+      <c r="M39" s="18" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="13" t="s">
+      <c r="A40" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B40" s="13" t="s">
+      <c r="B40" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="C40" s="13" t="s">
+      <c r="C40" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="D40" s="13" t="s">
+      <c r="D40" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="E40" s="13"/>
-      <c r="F40" s="13"/>
-      <c r="G40" s="13"/>
-      <c r="H40" s="13"/>
-      <c r="I40" s="13" t="s">
+      <c r="E40" s="12"/>
+      <c r="F40" s="12"/>
+      <c r="G40" s="12"/>
+      <c r="H40" s="12"/>
+      <c r="I40" s="12" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="13" t="s">
+      <c r="A41" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B41" s="13" t="s">
+      <c r="B41" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="C41" s="13" t="s">
+      <c r="C41" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="D41" s="13" t="s">
+      <c r="D41" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="E41" s="13"/>
-      <c r="F41" s="13"/>
-      <c r="G41" s="13"/>
-      <c r="H41" s="13"/>
-      <c r="I41" s="13" t="s">
+      <c r="E41" s="12"/>
+      <c r="F41" s="12"/>
+      <c r="G41" s="12"/>
+      <c r="H41" s="12"/>
+      <c r="I41" s="12" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="13" t="s">
+      <c r="A42" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B42" s="13" t="s">
+      <c r="B42" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="C42" s="13" t="s">
+      <c r="C42" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="D42" s="13" t="s">
+      <c r="D42" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="E42" s="13"/>
-      <c r="F42" s="13"/>
-      <c r="G42" s="13"/>
-      <c r="H42" s="13"/>
-      <c r="I42" s="13" t="s">
+      <c r="E42" s="12"/>
+      <c r="F42" s="12"/>
+      <c r="G42" s="12"/>
+      <c r="H42" s="12"/>
+      <c r="I42" s="12" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="6" t="s">
+      <c r="A43" s="0" t="s">
         <v>22</v>
       </c>
     </row>
@@ -2684,12 +2631,12 @@
   <dimension ref="A1:J999"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.33"/>
@@ -2704,352 +2651,352 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="0" t="s">
         <v>118</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="0" t="s">
         <v>119</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="19" t="s">
         <v>120</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="0" t="s">
         <v>121</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="0" t="s">
         <v>122</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="0" t="s">
         <v>123</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="0" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="0" t="s">
         <v>124</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="20" t="s">
         <v>125</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="0" t="s">
         <v>126</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="0" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="0" t="s">
         <v>124</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="20" t="s">
         <v>128</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="0" t="s">
         <v>129</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="0" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="0" t="s">
         <v>131</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="0" t="s">
         <v>133</v>
       </c>
-      <c r="J5" s="22"/>
+      <c r="J5" s="21"/>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="0" t="s">
         <v>134</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="21" t="s">
         <v>135</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="0" t="s">
         <v>136</v>
       </c>
-      <c r="J6" s="22"/>
+      <c r="J6" s="21"/>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="0" t="s">
         <v>137</v>
       </c>
-      <c r="C7" s="22" t="s">
+      <c r="C7" s="21" t="s">
         <v>138</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="0" t="s">
         <v>139</v>
       </c>
-      <c r="J7" s="22"/>
+      <c r="J7" s="21"/>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="0" t="s">
         <v>140</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="21" t="s">
         <v>141</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="0" t="s">
         <v>142</v>
       </c>
-      <c r="J8" s="22"/>
+      <c r="J8" s="21"/>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="0" t="s">
         <v>143</v>
       </c>
-      <c r="C9" s="22" t="s">
+      <c r="C9" s="21" t="s">
         <v>144</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="0" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="0" t="s">
         <v>146</v>
       </c>
-      <c r="C10" s="22" t="s">
+      <c r="C10" s="21" t="s">
         <v>147</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="0" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C11" s="22"/>
+      <c r="C11" s="21"/>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="0" t="s">
         <v>149</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="0" t="s">
         <v>150</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="0" t="s">
         <v>151</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="0" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="0" t="s">
         <v>149</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="0" t="s">
         <v>153</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="0" t="s">
         <v>154</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="0" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="0" t="s">
         <v>149</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="0" t="s">
         <v>156</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="0" t="s">
         <v>157</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="0" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="0" t="s">
         <v>149</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="0" t="s">
         <v>159</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="0" t="s">
         <v>160</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="0" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="0" t="s">
         <v>149</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="0" t="s">
         <v>162</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="0" t="s">
         <v>163</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="0" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="0" t="s">
         <v>149</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="0" t="s">
         <v>165</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="0" t="s">
         <v>166</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D17" s="0" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="13" t="s">
+      <c r="A19" s="12" t="s">
         <v>168</v>
       </c>
-      <c r="B19" s="13" t="s">
+      <c r="B19" s="12" t="s">
         <v>169</v>
       </c>
-      <c r="C19" s="13" t="s">
+      <c r="C19" s="12" t="s">
         <v>170</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D19" s="0" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="13" t="s">
+      <c r="A20" s="12" t="s">
         <v>168</v>
       </c>
-      <c r="B20" s="13" t="s">
+      <c r="B20" s="12" t="s">
         <v>172</v>
       </c>
-      <c r="C20" s="13" t="s">
+      <c r="C20" s="12" t="s">
         <v>173</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D20" s="0" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="13" t="s">
+      <c r="A21" s="12" t="s">
         <v>168</v>
       </c>
-      <c r="B21" s="13" t="s">
+      <c r="B21" s="12" t="s">
         <v>175</v>
       </c>
-      <c r="C21" s="13" t="s">
+      <c r="C21" s="12" t="s">
         <v>176</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="D21" s="0" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="13" t="s">
+      <c r="A22" s="12" t="s">
         <v>168</v>
       </c>
-      <c r="B22" s="13" t="s">
+      <c r="B22" s="12" t="s">
         <v>146</v>
       </c>
-      <c r="C22" s="13" t="s">
+      <c r="C22" s="12" t="s">
         <v>147</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="D22" s="0" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="13" t="s">
+      <c r="A24" s="12" t="s">
         <v>178</v>
       </c>
-      <c r="B24" s="13" t="s">
+      <c r="B24" s="12" t="s">
         <v>179</v>
       </c>
-      <c r="C24" s="13" t="s">
+      <c r="C24" s="12" t="s">
         <v>180</v>
       </c>
-      <c r="D24" s="6" t="s">
+      <c r="D24" s="0" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="13" t="s">
+      <c r="A25" s="12" t="s">
         <v>178</v>
       </c>
-      <c r="B25" s="13" t="s">
+      <c r="B25" s="12" t="s">
         <v>181</v>
       </c>
-      <c r="C25" s="13" t="s">
+      <c r="C25" s="12" t="s">
         <v>182</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="D25" s="0" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="13" t="s">
+      <c r="A26" s="12" t="s">
         <v>178</v>
       </c>
-      <c r="B26" s="13" t="s">
+      <c r="B26" s="12" t="s">
         <v>183</v>
       </c>
-      <c r="C26" s="13" t="s">
+      <c r="C26" s="12" t="s">
         <v>184</v>
       </c>
-      <c r="D26" s="6" t="s">
+      <c r="D26" s="0" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="13" t="s">
+      <c r="A27" s="12" t="s">
         <v>178</v>
       </c>
-      <c r="B27" s="13" t="s">
+      <c r="B27" s="12" t="s">
         <v>186</v>
       </c>
-      <c r="C27" s="13" t="s">
+      <c r="C27" s="12" t="s">
         <v>187</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="D27" s="0" t="s">
         <v>188</v>
       </c>
     </row>
@@ -4044,12 +3991,12 @@
   <dimension ref="A1:D1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D33" activeCellId="0" sqref="D33"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="39.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="23.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="24.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="10.66"/>
@@ -4057,30 +4004,30 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="0" t="s">
         <v>189</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="0" t="s">
         <v>190</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="22" t="s">
         <v>191</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="23" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>193</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="0" t="s">
         <v>195</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="D2" s="24" t="s">
         <v>125</v>
       </c>
     </row>

</xml_diff>